<commit_message>
Revert fuzzywuzzymit try to rescue deployment
</commit_message>
<xml_diff>
--- a/evaluation/Quantum_harmonic_oscillator_evaluation.xlsx
+++ b/evaluation/Quantum_harmonic_oscillator_evaluation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D4C9FC-CBD0-49DA-9BF4-BE2D614890A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37AF170-D6DC-468D-AA5D-EDAFD4D3EB93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="16395" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -461,7 +461,7 @@
     <col min="2" max="2" width="24.86328125" customWidth="1"/>
     <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" customWidth="1"/>
     <col min="6" max="6" width="8.796875" customWidth="1"/>
     <col min="7" max="7" width="12.796875" customWidth="1"/>
   </cols>
@@ -500,7 +500,9 @@
         <v>2</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
@@ -602,19 +604,19 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
         <v>3</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
         <v>4</v>
       </c>
     </row>
@@ -625,14 +627,14 @@
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>4</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>1</v>
       </c>
       <c r="G9" s="1"/>
@@ -644,12 +646,12 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>2</v>
       </c>
       <c r="G10" s="1"/>
@@ -676,9 +678,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -689,12 +689,12 @@
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>4</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>2</v>
       </c>
       <c r="G13" s="1"/>

</xml_diff>